<commit_message>
simple http request to vehicles
</commit_message>
<xml_diff>
--- a/dummy-data/data-design.xlsx
+++ b/dummy-data/data-design.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="89">
   <si>
     <t>#</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -48,10 +48,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>VIN</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>mdInput with double-input-confirmation</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -72,10 +68,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ownedByOrg</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>md-checkbox</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -88,10 +80,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>scrapType</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>show different form</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -216,14 +204,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>operationApplied</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>vehicleCondition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>residualValue</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -272,10 +252,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>engineDisreplacement</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>md-radio with md-input for further info</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -309,6 +285,89 @@
   </si>
   <si>
     <t>misc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>isRemote</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dataTypeInDB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>obj</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boolean</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string but only number</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>obj</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>with 6 or 7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>with 16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>isToDeregister</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mofcomVType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>isOrg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>agent</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>conditionAtEntrance</t>
+  </si>
+  <si>
+    <t>number</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>displacement</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>includedInTheForm</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -658,24 +717,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="21.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.1796875" customWidth="1"/>
-    <col min="4" max="5" width="19.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="40.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.6328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="22.1796875" customWidth="1"/>
+    <col min="5" max="6" width="19.08984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="40.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.6328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -683,112 +743,136 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>88</v>
       </c>
       <c r="E1" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="F1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" t="s">
-        <v>54</v>
-      </c>
       <c r="I1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="J1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="K1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>79</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>81</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H3" t="s">
         <v>5</v>
       </c>
-      <c r="G3" t="s">
-        <v>20</v>
-      </c>
       <c r="I3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="K3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>82</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>81</v>
       </c>
       <c r="E4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="G4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -796,22 +880,28 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>81</v>
       </c>
       <c r="E5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F5" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="G5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="H5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -819,578 +909,745 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>81</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" t="s">
+        <v>72</v>
+      </c>
+      <c r="H6" t="s">
         <v>5</v>
       </c>
-      <c r="G6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>81</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="G7" t="s">
+        <v>72</v>
+      </c>
+      <c r="H7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>81</v>
       </c>
       <c r="E8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" t="s">
+        <v>72</v>
+      </c>
+      <c r="H8" t="s">
         <v>4</v>
       </c>
-      <c r="I8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>81</v>
+      </c>
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" t="s">
+        <v>76</v>
+      </c>
+      <c r="H9" t="s">
+        <v>3</v>
+      </c>
+      <c r="I9" t="s">
         <v>38</v>
       </c>
-      <c r="C9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" t="s">
-        <v>3</v>
-      </c>
-      <c r="G9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" t="s">
+        <v>76</v>
+      </c>
+      <c r="H10" t="s">
+        <v>3</v>
+      </c>
+      <c r="I10" t="s">
         <v>39</v>
       </c>
-      <c r="C10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" t="s">
-        <v>30</v>
-      </c>
-      <c r="F10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>81</v>
       </c>
       <c r="E11" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="G11" t="s">
+        <v>70</v>
+      </c>
+      <c r="H11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>33</v>
+        <v>81</v>
       </c>
       <c r="E12" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="G12" t="s">
+        <v>70</v>
+      </c>
+      <c r="H12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" t="s">
+        <v>74</v>
+      </c>
+      <c r="H13" t="s">
+        <v>3</v>
+      </c>
+      <c r="I13" t="s">
         <v>40</v>
       </c>
-      <c r="C13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D14" t="s">
-        <v>30</v>
+        <v>81</v>
       </c>
       <c r="E14" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F14" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" t="s">
+        <v>72</v>
+      </c>
+      <c r="H14" t="s">
         <v>5</v>
       </c>
-      <c r="G14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D15" t="s">
-        <v>30</v>
+        <v>81</v>
       </c>
       <c r="E15" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F15" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="G15" t="s">
+        <v>72</v>
+      </c>
+      <c r="H15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D16" t="s">
-        <v>30</v>
+        <v>81</v>
       </c>
       <c r="E16" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F16" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="G16" t="s">
+        <v>70</v>
+      </c>
+      <c r="H16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C17" t="s">
-        <v>13</v>
+        <v>83</v>
       </c>
       <c r="D17" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="E17" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="G17" t="s">
+        <v>75</v>
+      </c>
+      <c r="H17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C18" t="s">
-        <v>13</v>
+        <v>83</v>
       </c>
       <c r="D18" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="E18" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F18" t="s">
-        <v>3</v>
+        <v>57</v>
       </c>
       <c r="G18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="H18" t="s">
+        <v>3</v>
+      </c>
+      <c r="I18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C19" t="s">
-        <v>13</v>
+        <v>83</v>
       </c>
       <c r="D19" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="E19" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F19" t="s">
-        <v>3</v>
+        <v>57</v>
       </c>
       <c r="G19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="H19" t="s">
+        <v>3</v>
+      </c>
+      <c r="I19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>50</v>
+        <v>78</v>
       </c>
       <c r="C20" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" t="s">
+        <v>81</v>
+      </c>
+      <c r="E20" t="s">
+        <v>58</v>
+      </c>
+      <c r="F20" t="s">
+        <v>28</v>
+      </c>
+      <c r="G20" t="s">
         <v>73</v>
       </c>
-      <c r="D20" t="s">
-        <v>63</v>
-      </c>
-      <c r="E20" t="s">
-        <v>31</v>
-      </c>
-      <c r="F20" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C21" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D21" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="E21" t="s">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="F21" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="G21" t="s">
+        <v>72</v>
+      </c>
+      <c r="H21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>51</v>
+        <v>84</v>
       </c>
       <c r="C22" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D22" t="s">
-        <v>33</v>
+        <v>81</v>
       </c>
       <c r="E22" t="s">
         <v>30</v>
       </c>
       <c r="F22" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="G22" t="s">
+        <v>70</v>
+      </c>
+      <c r="H22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C23" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D23" t="s">
-        <v>33</v>
+        <v>81</v>
       </c>
       <c r="E23" t="s">
         <v>30</v>
       </c>
       <c r="F23" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="G23" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="H23" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="I23" t="s">
+        <v>48</v>
+      </c>
+      <c r="J23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C24" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D24" t="s">
-        <v>30</v>
+        <v>81</v>
       </c>
       <c r="E24" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F24" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="G24" t="s">
+        <v>70</v>
+      </c>
+      <c r="H24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C25" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D25" t="s">
-        <v>33</v>
+        <v>81</v>
       </c>
       <c r="E25" t="s">
         <v>30</v>
       </c>
       <c r="F25" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="G25" t="s">
+        <v>70</v>
+      </c>
+      <c r="H25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C26" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D26" t="s">
-        <v>30</v>
+        <v>81</v>
       </c>
       <c r="E26" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F26" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="G26" t="s">
+        <v>86</v>
+      </c>
+      <c r="H26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27" t="s">
+        <v>81</v>
+      </c>
+      <c r="E27" t="s">
+        <v>27</v>
+      </c>
+      <c r="F27" t="s">
+        <v>55</v>
+      </c>
+      <c r="H27" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" t="s">
+        <v>81</v>
+      </c>
+      <c r="E28" t="s">
+        <v>30</v>
+      </c>
+      <c r="F28" t="s">
+        <v>27</v>
+      </c>
+      <c r="H28" t="s">
         <v>59</v>
       </c>
-      <c r="C27" t="s">
-        <v>36</v>
-      </c>
-      <c r="D27" t="s">
-        <v>30</v>
-      </c>
-      <c r="E27" t="s">
-        <v>60</v>
-      </c>
-      <c r="F27" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28" t="s">
-        <v>61</v>
-      </c>
-      <c r="C28" t="s">
-        <v>36</v>
-      </c>
-      <c r="D28" t="s">
-        <v>33</v>
-      </c>
-      <c r="E28" t="s">
-        <v>30</v>
-      </c>
-      <c r="F28" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="C29" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D29" t="s">
-        <v>33</v>
+        <v>81</v>
       </c>
       <c r="E29" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F29" t="s">
-        <v>3</v>
-      </c>
-      <c r="G29" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="H29" t="s">
+        <v>3</v>
+      </c>
+      <c r="I29" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C30" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D30" t="s">
-        <v>30</v>
+        <v>81</v>
       </c>
       <c r="E30" t="s">
+        <v>27</v>
+      </c>
+      <c r="F30" t="s">
+        <v>30</v>
+      </c>
+      <c r="H30" t="s">
+        <v>3</v>
+      </c>
+      <c r="I30" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" t="s">
         <v>33</v>
       </c>
-      <c r="F30" t="s">
-        <v>3</v>
-      </c>
-      <c r="G30" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="B31" t="s">
-        <v>71</v>
-      </c>
-      <c r="C31" t="s">
-        <v>36</v>
-      </c>
       <c r="D31" t="s">
-        <v>30</v>
+        <v>81</v>
       </c>
       <c r="E31" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F31" t="s">
-        <v>3</v>
-      </c>
-      <c r="G31" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="H31" t="s">
+        <v>3</v>
+      </c>
+      <c r="I31" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C32" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D32" t="s">
-        <v>30</v>
+        <v>81</v>
       </c>
       <c r="E32" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F32" t="s">
-        <v>3</v>
-      </c>
-      <c r="G32" t="s">
-        <v>70</v>
+        <v>30</v>
+      </c>
+      <c r="H32" t="s">
+        <v>3</v>
+      </c>
+      <c r="I32" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33" t="s">
+        <v>81</v>
+      </c>
+      <c r="E33" t="s">
+        <v>27</v>
+      </c>
+      <c r="F33" t="s">
+        <v>30</v>
+      </c>
+      <c r="H33" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>